<commit_message>
looking at tracer data for floods (downstream)
</commit_message>
<xml_diff>
--- a/Hydrophones/Calibration/flow_experiment_tracers.xlsx
+++ b/Hydrophones/Calibration/flow_experiment_tracers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huck4481\Documents\GitHub\La_Jara\Hydrophones\Calibration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Documents\GitHub\La_Jara\Hydrophones\Calibration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B81C1E90-CA61-4213-8511-691E4F8806B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FEA694F-F7D2-447D-8461-9F9A7786B2A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B073A66E-6BB5-492B-8275-ACCE89EFB9F4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B073A66E-6BB5-492B-8275-ACCE89EFB9F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Flood1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="30">
   <si>
     <t>Tracer ID</t>
   </si>
@@ -111,6 +111,21 @@
   </si>
   <si>
     <t>% Tracers Moved</t>
+  </si>
+  <si>
+    <t>Flood 1</t>
+  </si>
+  <si>
+    <t>Flood 2</t>
+  </si>
+  <si>
+    <t>Flood 3</t>
+  </si>
+  <si>
+    <t>Flood 4</t>
+  </si>
+  <si>
+    <t>Flood 5</t>
   </si>
 </sst>
 </file>
@@ -200,12 +215,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -214,16 +229,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -232,13 +247,19 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -583,30 +604,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D864ED87-307D-4916-B61D-7A986C44CDD6}">
-  <dimension ref="A1:R69"/>
+  <dimension ref="A1:S69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+    <sheetView tabSelected="1" topLeftCell="E22" workbookViewId="0">
+      <selection activeCell="S36" sqref="S36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="10.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="1"/>
-    <col min="5" max="5" width="16.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="18.85546875" style="1" customWidth="1"/>
+    <col min="1" max="2" width="9.109375" style="1"/>
+    <col min="3" max="3" width="10.109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.109375" style="1"/>
+    <col min="5" max="5" width="16.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18.88671875" style="1" customWidth="1"/>
     <col min="7" max="7" width="17" customWidth="1"/>
-    <col min="8" max="8" width="18.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="18.5703125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="11" customWidth="1"/>
-    <col min="15" max="15" width="13.140625" customWidth="1"/>
-    <col min="16" max="16" width="14" customWidth="1"/>
-    <col min="17" max="17" width="14.28515625" customWidth="1"/>
-    <col min="18" max="18" width="15.28515625" customWidth="1"/>
+    <col min="8" max="8" width="18.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="18.5546875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="8.88671875" style="1"/>
+    <col min="12" max="12" width="11" style="1" customWidth="1"/>
+    <col min="13" max="14" width="8.88671875" style="1"/>
+    <col min="15" max="15" width="13.109375" style="1" customWidth="1"/>
+    <col min="16" max="16" width="14" style="1" customWidth="1"/>
+    <col min="17" max="17" width="14.33203125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="15.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -635,7 +658,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
         <v>7</v>
       </c>
@@ -663,8 +686,18 @@
       <c r="I2" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="K2" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
+      <c r="P2" s="13"/>
+      <c r="Q2" s="13"/>
+      <c r="R2" s="13"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="11">
         <v>151</v>
       </c>
@@ -717,7 +750,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>89</v>
       </c>
@@ -752,11 +785,28 @@
         <v>128</v>
       </c>
       <c r="M4" s="1">
-        <f>COUNTIF(B2:B68,"o")</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+        <f>COUNTIF($B$2:$B$68,"o")</f>
+        <v>5</v>
+      </c>
+      <c r="N4" s="1">
+        <f>COUNTIFS($B$2:$B$66,"o", $E$2:$E$66,"&lt;&gt;0")</f>
+        <v>0</v>
+      </c>
+      <c r="O4" s="1">
+        <v>0</v>
+      </c>
+      <c r="P4" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>0</v>
+      </c>
+      <c r="R4" s="14">
+        <f>N4/M4*100</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>149</v>
       </c>
@@ -791,11 +841,32 @@
         <v>90</v>
       </c>
       <c r="M5" s="1">
-        <f>COUNTIF(B2:B68,"w")</f>
+        <f>COUNTIF($B$2:$B$68,"w")</f>
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="N5" s="1">
+        <f>COUNTIFS($B$2:$B$66,"w", $E$2:$E$66,"&lt;&gt;0")</f>
+        <v>1</v>
+      </c>
+      <c r="O5" s="1">
+        <f>AVERAGEIFS($E$2:$E$66, $B$2:$B$66, "w", $E$2:$E$66, "&lt;&gt;0")</f>
+        <v>102</v>
+      </c>
+      <c r="P5" s="1">
+        <f>_xlfn.MINIFS($E$2:$E$66, $B$2:$B$66, "w", $E$2:$E$66, "&lt;&gt;0")</f>
+        <v>102</v>
+      </c>
+      <c r="Q5" s="1">
+        <f>_xlfn.MAXIFS($E$2:$E$66, $B$2:$B$66, "w", $E$2:$E$66, "&lt;&gt;0")</f>
+        <v>102</v>
+      </c>
+      <c r="R5" s="14">
+        <f t="shared" ref="R5:R9" si="0">N5/M5*100</f>
+        <v>12.5</v>
+      </c>
+      <c r="S5" s="1"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>23</v>
       </c>
@@ -830,11 +901,32 @@
         <v>64</v>
       </c>
       <c r="M6" s="1">
-        <f>COUNTIF(B2:B68,"p")</f>
+        <f>COUNTIF($B$2:$B$68,"p")</f>
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="N6" s="1">
+        <f>COUNTIFS($B$2:$B$66,"p", $E$2:$E$66,"&lt;&gt;0")</f>
+        <v>2</v>
+      </c>
+      <c r="O6" s="1">
+        <f>AVERAGEIFS($E$2:$E$66, $B$2:$B$66, "p", $E$2:$E$66, "&lt;&gt;0")</f>
+        <v>18</v>
+      </c>
+      <c r="P6" s="1">
+        <f>_xlfn.MINIFS($E$2:$E$66, $B$2:$B$66, "p", $E$2:$E$66, "&lt;&gt;0")</f>
+        <v>12</v>
+      </c>
+      <c r="Q6" s="1">
+        <f>_xlfn.MAXIFS($E$2:$E$66, $B$2:$B$66, "p", $E$2:$E$66, "&lt;&gt;0")</f>
+        <v>24</v>
+      </c>
+      <c r="R6" s="14">
+        <f t="shared" si="0"/>
+        <v>14.285714285714285</v>
+      </c>
+      <c r="S6" s="1"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>158</v>
       </c>
@@ -869,11 +961,32 @@
         <v>45</v>
       </c>
       <c r="M7" s="1">
-        <f>COUNTIF(B2:B68,"g")</f>
+        <f>COUNTIF($B$2:$B$68,"g")</f>
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="N7" s="1">
+        <f>COUNTIFS($B$2:$B$66,"g", $E$2:$E$66,"&lt;&gt;0")</f>
+        <v>2</v>
+      </c>
+      <c r="O7" s="1">
+        <f>AVERAGEIFS($E$2:$E$66, $B$2:$B$66, "g", $E$2:$E$66, "&lt;&gt;0")</f>
+        <v>15</v>
+      </c>
+      <c r="P7" s="1">
+        <f>_xlfn.MINIFS($E$2:$E$66, $B$2:$B$66, "g", $E$2:$E$66, "&lt;&gt;0")</f>
+        <v>3</v>
+      </c>
+      <c r="Q7" s="1">
+        <f>_xlfn.MAXIFS($E$2:$E$66, $B$2:$B$66, "g", $E$2:$E$66, "&lt;&gt;0")</f>
+        <v>27</v>
+      </c>
+      <c r="R7" s="14">
+        <f t="shared" si="0"/>
+        <v>12.5</v>
+      </c>
+      <c r="S7" s="1"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="11">
         <v>157</v>
       </c>
@@ -908,11 +1021,32 @@
         <v>32</v>
       </c>
       <c r="M8" s="1">
-        <f>COUNTIF(B2:B68,"y")</f>
+        <f>COUNTIF($B$2:$B$68,"y")</f>
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="N8" s="1">
+        <f>COUNTIFS($B$2:$B$66,"y", $E$2:$E$66,"&lt;&gt;0")</f>
+        <v>5</v>
+      </c>
+      <c r="O8" s="1">
+        <f>AVERAGEIFS($E$2:$E$66, $B$2:$B$66, "y", $E$2:$E$66, "&lt;&gt;0")</f>
+        <v>19.3</v>
+      </c>
+      <c r="P8" s="1">
+        <f>_xlfn.MINIFS($E$2:$E$66, $B$2:$B$66, "y", $E$2:$E$66, "&lt;&gt;0")</f>
+        <v>4</v>
+      </c>
+      <c r="Q8" s="1">
+        <f>_xlfn.MAXIFS($E$2:$E$66, $B$2:$B$66, "y", $E$2:$E$66, "&lt;&gt;0")</f>
+        <v>36.5</v>
+      </c>
+      <c r="R8" s="14">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="S8" s="1"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>141</v>
       </c>
@@ -940,18 +1074,39 @@
       <c r="I9" s="7">
         <v>40</v>
       </c>
-      <c r="K9" s="13" t="s">
+      <c r="K9" s="12" t="s">
         <v>7</v>
       </c>
       <c r="L9" s="1">
         <v>16</v>
       </c>
       <c r="M9" s="1">
-        <f>COUNTIF(B2:B68,"r")</f>
+        <f>COUNTIF($B$2:$B$68,"r")</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="N9" s="1">
+        <f>COUNTIFS($B$2:$B$66,"r", $E$2:$E$66,"&lt;&gt;0")</f>
+        <v>1</v>
+      </c>
+      <c r="O9" s="1">
+        <f>AVERAGEIFS($E$2:$E$66, $B$2:$B$66, "r", $E$2:$E$66, "&lt;&gt;0")</f>
+        <v>16</v>
+      </c>
+      <c r="P9" s="1">
+        <f>_xlfn.MINIFS($E$2:$E$66, $B$2:$B$66, "r", $E$2:$E$66, "&lt;&gt;0")</f>
+        <v>16</v>
+      </c>
+      <c r="Q9" s="1">
+        <f>_xlfn.MAXIFS($E$2:$E$66, $B$2:$B$66, "r", $E$2:$E$66, "&lt;&gt;0")</f>
+        <v>16</v>
+      </c>
+      <c r="R9" s="14">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="S9" s="1"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>163</v>
       </c>
@@ -980,7 +1135,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
         <v>170</v>
       </c>
@@ -1008,8 +1163,18 @@
       <c r="I11" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="K11" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="L11" s="13"/>
+      <c r="M11" s="13"/>
+      <c r="N11" s="13"/>
+      <c r="O11" s="13"/>
+      <c r="P11" s="13"/>
+      <c r="Q11" s="13"/>
+      <c r="R11" s="13"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="9">
         <v>167</v>
       </c>
@@ -1037,8 +1202,32 @@
       <c r="I12" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="K12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R12" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>101</v>
       </c>
@@ -1066,8 +1255,35 @@
       <c r="I13" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="K13" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="L13" s="1">
+        <v>128</v>
+      </c>
+      <c r="M13" s="1">
+        <f>COUNTIF($B$2:$B$68,"o")</f>
+        <v>5</v>
+      </c>
+      <c r="N13" s="1">
+        <f>COUNTIFS($B$2:$B$66,"o", $F$2:$F$66,"&lt;&gt;0")</f>
+        <v>0</v>
+      </c>
+      <c r="O13" s="1">
+        <v>0</v>
+      </c>
+      <c r="P13" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="1">
+        <v>0</v>
+      </c>
+      <c r="R13" s="14">
+        <f>N13/M13*100</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>35</v>
       </c>
@@ -1095,8 +1311,38 @@
       <c r="I14" s="2">
         <v>21</v>
       </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="K14" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="L14" s="1">
+        <v>90</v>
+      </c>
+      <c r="M14" s="1">
+        <f>COUNTIF($B$2:$B$68,"w")</f>
+        <v>8</v>
+      </c>
+      <c r="N14" s="1">
+        <f>COUNTIFS($B$2:$B$66,"w", $F$2:$F$66,"&lt;&gt;0")</f>
+        <v>2</v>
+      </c>
+      <c r="O14" s="1">
+        <f>AVERAGEIFS($F2:$F66, $B$2:$B$66, "w", $F2:$F66, "&lt;&gt;0")</f>
+        <v>13</v>
+      </c>
+      <c r="P14" s="1">
+        <f>_xlfn.MINIFS($F2:$F66, $B$2:$B$66, "w", $F2:$F66, "&lt;&gt;0")</f>
+        <v>7</v>
+      </c>
+      <c r="Q14" s="1">
+        <f>_xlfn.MAXIFS($F2:$F66, $B$2:$B$66, "w", $F2:$F66, "&lt;&gt;0")</f>
+        <v>19</v>
+      </c>
+      <c r="R14" s="14">
+        <f t="shared" ref="R14:R18" si="1">N14/M14*100</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="7">
         <v>52</v>
       </c>
@@ -1124,8 +1370,38 @@
       <c r="I15" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="K15" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="L15" s="1">
+        <v>64</v>
+      </c>
+      <c r="M15" s="1">
+        <f>COUNTIF($B$2:$B$68,"p")</f>
+        <v>14</v>
+      </c>
+      <c r="N15" s="1">
+        <f>COUNTIFS($B$2:$B$66,"p", $F$2:$F$66,"&lt;&gt;0")</f>
+        <v>4</v>
+      </c>
+      <c r="O15" s="1">
+        <f>AVERAGEIFS($F$2:$F$66, $B$2:$B$66, "p", $F$2:$F$66, "&lt;&gt;0")</f>
+        <v>23.75</v>
+      </c>
+      <c r="P15" s="1">
+        <f>_xlfn.MINIFS($F$2:$F$66, $B$2:$B$66, "p", $F$2:$F$66, "&lt;&gt;0")</f>
+        <v>13</v>
+      </c>
+      <c r="Q15" s="1">
+        <f>_xlfn.MAXIFS($F$2:$F$66, $B$2:$B$66, "p", $F$2:$F$66, "&lt;&gt;0")</f>
+        <v>43</v>
+      </c>
+      <c r="R15" s="14">
+        <f t="shared" si="1"/>
+        <v>28.571428571428569</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="7">
         <v>146</v>
       </c>
@@ -1153,8 +1429,38 @@
       <c r="I16" s="7">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L16" s="1">
+        <v>45</v>
+      </c>
+      <c r="M16" s="1">
+        <f>COUNTIF($B$2:$B$68,"g")</f>
+        <v>16</v>
+      </c>
+      <c r="N16" s="1">
+        <f>COUNTIFS($B$2:$B$66,"g", $F$2:$F$66,"&lt;&gt;0")</f>
+        <v>5</v>
+      </c>
+      <c r="O16" s="1">
+        <f>AVERAGEIFS($F$2:$F$66, $B$2:$B$66, "g", $F$2:$F$66, "&lt;&gt;0")</f>
+        <v>24.8</v>
+      </c>
+      <c r="P16" s="1">
+        <f>_xlfn.MINIFS($F$2:$F$66, $B$2:$B$66, "g", $F$2:$F$66, "&lt;&gt;0")</f>
+        <v>5</v>
+      </c>
+      <c r="Q16" s="1">
+        <f>_xlfn.MAXIFS($F$2:$F$66, $B$2:$B$66, "g", $F$2:$F$66, "&lt;&gt;0")</f>
+        <v>50</v>
+      </c>
+      <c r="R16" s="14">
+        <f t="shared" si="1"/>
+        <v>31.25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" s="11">
         <v>156</v>
       </c>
@@ -1182,8 +1488,38 @@
       <c r="I17" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K17" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="L17" s="1">
+        <v>32</v>
+      </c>
+      <c r="M17" s="1">
+        <f>COUNTIF($B$2:$B$68,"y")</f>
+        <v>20</v>
+      </c>
+      <c r="N17" s="1">
+        <f>COUNTIFS($B$2:$B$66,"y", $F$2:$F$66,"&lt;&gt;0")</f>
+        <v>8</v>
+      </c>
+      <c r="O17" s="1">
+        <f>AVERAGEIFS($F$2:$F$66, $B$2:$B$66, "y", $F$2:$F$66, "&lt;&gt;0")</f>
+        <v>55</v>
+      </c>
+      <c r="P17" s="1">
+        <f>_xlfn.MINIFS($F$2:$F$66, $B$2:$B$66, "y", $F$2:$F$66, "&lt;&gt;0")</f>
+        <v>5</v>
+      </c>
+      <c r="Q17" s="1">
+        <f>_xlfn.MAXIFS($F$2:$F$66, $B$2:$B$66, "y", $F$2:$F$66, "&lt;&gt;0")</f>
+        <v>140</v>
+      </c>
+      <c r="R17" s="14">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
         <v>97</v>
       </c>
@@ -1211,8 +1547,38 @@
       <c r="I18" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K18" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="L18" s="1">
+        <v>16</v>
+      </c>
+      <c r="M18" s="1">
+        <f>COUNTIF($B$2:$B$68,"r")</f>
+        <v>2</v>
+      </c>
+      <c r="N18" s="1">
+        <f>COUNTIFS($B$2:$B$66,"r", $F$2:$F$66,"&lt;&gt;0")</f>
+        <v>1</v>
+      </c>
+      <c r="O18" s="1">
+        <f>AVERAGEIFS($F$2:$F$66, $B$2:$B$66, "r", $F$2:$F$66, "&lt;&gt;0")</f>
+        <v>41</v>
+      </c>
+      <c r="P18" s="1">
+        <f>_xlfn.MINIFS($F$2:$F$66, $B$2:$B$66, "r", $F$2:$F$66, "&lt;&gt;0")</f>
+        <v>41</v>
+      </c>
+      <c r="Q18" s="1">
+        <f>_xlfn.MAXIFS($F$2:$F$66, $B$2:$B$66, "r", $F$2:$F$66, "&lt;&gt;0")</f>
+        <v>41</v>
+      </c>
+      <c r="R18" s="14">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>162</v>
       </c>
@@ -1241,7 +1607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" s="7">
         <v>65</v>
       </c>
@@ -1269,8 +1635,18 @@
       <c r="I20" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K20" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="L20" s="13"/>
+      <c r="M20" s="13"/>
+      <c r="N20" s="13"/>
+      <c r="O20" s="13"/>
+      <c r="P20" s="13"/>
+      <c r="Q20" s="13"/>
+      <c r="R20" s="13"/>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21" s="7">
         <v>133</v>
       </c>
@@ -1298,8 +1674,32 @@
       <c r="I21" s="7">
         <v>7</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R21" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" s="6">
         <v>111</v>
       </c>
@@ -1327,8 +1727,35 @@
       <c r="I22" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K22" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="L22" s="1">
+        <v>128</v>
+      </c>
+      <c r="M22" s="1">
+        <f>COUNTIF($B$2:$B$68,"o")</f>
+        <v>5</v>
+      </c>
+      <c r="N22" s="1">
+        <f>COUNTIFS($B$2:$B$66,"o", $G$2:$G$66,"&lt;&gt;0")</f>
+        <v>0</v>
+      </c>
+      <c r="O22" s="1">
+        <v>0</v>
+      </c>
+      <c r="P22" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="1">
+        <v>0</v>
+      </c>
+      <c r="R22" s="14">
+        <f>N22/M22*100</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" s="9">
         <v>6</v>
       </c>
@@ -1356,8 +1783,35 @@
       <c r="I23" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K23" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="L23" s="1">
+        <v>90</v>
+      </c>
+      <c r="M23" s="1">
+        <f>COUNTIF($B$2:$B$68,"w")</f>
+        <v>8</v>
+      </c>
+      <c r="N23" s="1">
+        <f>COUNTIFS($B$2:$B$66,"w", $G$2:$G$66,"&lt;&gt;0")</f>
+        <v>0</v>
+      </c>
+      <c r="O23" s="1">
+        <v>0</v>
+      </c>
+      <c r="P23" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="1">
+        <v>0</v>
+      </c>
+      <c r="R23" s="14">
+        <f t="shared" ref="R23:R27" si="2">N23/M23*100</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>100</v>
       </c>
@@ -1385,8 +1839,35 @@
       <c r="I24" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K24" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="L24" s="1">
+        <v>64</v>
+      </c>
+      <c r="M24" s="1">
+        <f>COUNTIF($B$2:$B$68,"p")</f>
+        <v>14</v>
+      </c>
+      <c r="N24" s="1">
+        <f>COUNTIFS($B$2:$B$66,"p", $G$2:$G$66,"&lt;&gt;0")</f>
+        <v>0</v>
+      </c>
+      <c r="O24" s="1">
+        <v>0</v>
+      </c>
+      <c r="P24" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="1">
+        <v>0</v>
+      </c>
+      <c r="R24" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" s="7">
         <v>127</v>
       </c>
@@ -1414,8 +1895,38 @@
       <c r="I25" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K25" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L25" s="1">
+        <v>45</v>
+      </c>
+      <c r="M25" s="1">
+        <f>COUNTIF($B$2:$B$68,"g")</f>
+        <v>16</v>
+      </c>
+      <c r="N25" s="1">
+        <f>COUNTIFS($B$2:$B$66,"g", $G$2:$G$66,"&lt;&gt;0")</f>
+        <v>3</v>
+      </c>
+      <c r="O25" s="1">
+        <f>AVERAGEIFS($G$2:$G$66, $B$2:$B$66, "g", $G$2:$G$66, "&lt;&gt;0")</f>
+        <v>38</v>
+      </c>
+      <c r="P25" s="1">
+        <f>_xlfn.MINIFS($G$2:$G$66, $B$2:$B$66, "g", $G$2:$G$66, "&lt;&gt;0")</f>
+        <v>12</v>
+      </c>
+      <c r="Q25" s="1">
+        <f>_xlfn.MAXIFS($G$2:$G$66, $B$2:$B$66, "g", $G$2:$G$66, "&lt;&gt;0")</f>
+        <v>59</v>
+      </c>
+      <c r="R25" s="14">
+        <f t="shared" si="2"/>
+        <v>18.75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26" s="7">
         <v>53</v>
       </c>
@@ -1443,8 +1954,38 @@
       <c r="I26" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K26" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="L26" s="1">
+        <v>32</v>
+      </c>
+      <c r="M26" s="1">
+        <f>COUNTIF($B$2:$B$68,"y")</f>
+        <v>20</v>
+      </c>
+      <c r="N26" s="1">
+        <f>COUNTIFS($B$2:$B$66,"y", $G$2:$G$66,"&lt;&gt;0")</f>
+        <v>4</v>
+      </c>
+      <c r="O26" s="1">
+        <f>AVERAGEIFS($G$2:$G$66, $B$2:$B$66, "y", $G$2:$G$66, "&lt;&gt;0")</f>
+        <v>35.5</v>
+      </c>
+      <c r="P26" s="1">
+        <f>_xlfn.MINIFS($G$2:$G$66, $B$2:$B$66, "y", $G$2:$G$66, "&lt;&gt;0")</f>
+        <v>10</v>
+      </c>
+      <c r="Q26" s="1">
+        <f>_xlfn.MAXIFS($G$2:$G$66, $B$2:$B$66, "y", $G$2:$G$66, "&lt;&gt;0")</f>
+        <v>96</v>
+      </c>
+      <c r="R26" s="14">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A27" s="11">
         <v>22</v>
       </c>
@@ -1472,8 +2013,38 @@
       <c r="I27" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K27" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="L27" s="1">
+        <v>16</v>
+      </c>
+      <c r="M27" s="1">
+        <f>COUNTIF($B$2:$B$68,"r")</f>
+        <v>2</v>
+      </c>
+      <c r="N27" s="1">
+        <f>COUNTIFS($B$2:$B$66,"r", $G$2:$G$66,"&lt;&gt;0")</f>
+        <v>1</v>
+      </c>
+      <c r="O27" s="1">
+        <f>AVERAGEIFS($G$2:$G$66, $B$2:$B$66, "r", $G$2:$G$66, "&lt;&gt;0")</f>
+        <v>101</v>
+      </c>
+      <c r="P27" s="1">
+        <f>_xlfn.MINIFS($G$2:$G$66, $B$2:$B$66, "r", $G$2:$G$66, "&lt;&gt;0")</f>
+        <v>101</v>
+      </c>
+      <c r="Q27" s="1">
+        <f>_xlfn.MAXIFS($G$2:$G$66, $B$2:$B$66, "r", $G$2:$G$66, "&lt;&gt;0")</f>
+        <v>101</v>
+      </c>
+      <c r="R27" s="14">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28" s="5">
         <v>99</v>
       </c>
@@ -1502,7 +2073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>38</v>
       </c>
@@ -1530,8 +2101,18 @@
       <c r="I29" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K29" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="L29" s="13"/>
+      <c r="M29" s="13"/>
+      <c r="N29" s="13"/>
+      <c r="O29" s="13"/>
+      <c r="P29" s="13"/>
+      <c r="Q29" s="13"/>
+      <c r="R29" s="13"/>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A30" s="7">
         <v>135</v>
       </c>
@@ -1559,8 +2140,32 @@
       <c r="I30" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K30" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M30" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N30" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O30" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P30" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q30" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R30" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A31" s="12">
         <v>166</v>
       </c>
@@ -1588,8 +2193,35 @@
       <c r="I31" s="12">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K31" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="L31" s="1">
+        <v>128</v>
+      </c>
+      <c r="M31" s="1">
+        <f>COUNTIF($B$2:$B$68,"o")</f>
+        <v>5</v>
+      </c>
+      <c r="N31" s="1">
+        <f>COUNTIFS($B$2:$B$66,"o", $H$2:$H$66,"&lt;&gt;0")</f>
+        <v>0</v>
+      </c>
+      <c r="O31" s="1">
+        <v>0</v>
+      </c>
+      <c r="P31" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="1">
+        <v>0</v>
+      </c>
+      <c r="R31" s="14">
+        <f>N31/M31*100</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A32" s="5">
         <v>29</v>
       </c>
@@ -1617,8 +2249,35 @@
       <c r="I32" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K32" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="L32" s="1">
+        <v>90</v>
+      </c>
+      <c r="M32" s="1">
+        <f>COUNTIF($B$2:$B$68,"w")</f>
+        <v>8</v>
+      </c>
+      <c r="N32" s="1">
+        <f>COUNTIFS($B$2:$B$66,"w", $H$2:$H$66,"&lt;&gt;0")</f>
+        <v>0</v>
+      </c>
+      <c r="O32" s="1">
+        <v>0</v>
+      </c>
+      <c r="P32" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q32" s="1">
+        <v>0</v>
+      </c>
+      <c r="R32" s="14">
+        <f t="shared" ref="R32:R36" si="3">N32/M32*100</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>160</v>
       </c>
@@ -1646,8 +2305,38 @@
       <c r="I33" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K33" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="L33" s="1">
+        <v>64</v>
+      </c>
+      <c r="M33" s="1">
+        <f>COUNTIF($B$2:$B$68,"p")</f>
+        <v>14</v>
+      </c>
+      <c r="N33" s="1">
+        <f>COUNTIFS($B$2:$B$66,"p", $H$2:$H$66,"&lt;&gt;0")</f>
+        <v>1</v>
+      </c>
+      <c r="O33" s="1">
+        <f>AVERAGEIFS($H$2:$H$66, $B$2:$B$66, "p", $H$2:$H$66, "&lt;&gt;0")</f>
+        <v>30</v>
+      </c>
+      <c r="P33" s="1">
+        <f>_xlfn.MINIFS($H$2:$H$66, $B$2:$B$66, "p", $H$2:$H$66, "&lt;&gt;0")</f>
+        <v>30</v>
+      </c>
+      <c r="Q33" s="1">
+        <f>_xlfn.MAXIFS($H$2:$H$66, $B$2:$B$66, "p", $H$2:$H$66, "&lt;&gt;0")</f>
+        <v>30</v>
+      </c>
+      <c r="R33" s="14">
+        <f t="shared" si="3"/>
+        <v>7.1428571428571423</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A34" s="11">
         <v>155</v>
       </c>
@@ -1675,8 +2364,38 @@
       <c r="I34" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K34" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L34" s="1">
+        <v>45</v>
+      </c>
+      <c r="M34" s="1">
+        <f>COUNTIF($B$2:$B$68,"g")</f>
+        <v>16</v>
+      </c>
+      <c r="N34" s="1">
+        <f>COUNTIFS($B$2:$B$66,"g", $H$2:$H$66,"&lt;&gt;0")</f>
+        <v>4</v>
+      </c>
+      <c r="O34" s="1">
+        <f>AVERAGEIFS($H$2:$H$66, $B$2:$B$66, "g", $H$2:$H$66, "&lt;&gt;0")</f>
+        <v>55.25</v>
+      </c>
+      <c r="P34" s="1">
+        <f>_xlfn.MINIFS($H$2:$H$66, $B$2:$B$66, "g", $H$2:$H$66, "&lt;&gt;0")</f>
+        <v>10</v>
+      </c>
+      <c r="Q34" s="1">
+        <f>_xlfn.MAXIFS($H$2:$H$66, $B$2:$B$66, "g", $H$2:$H$66, "&lt;&gt;0")</f>
+        <v>116</v>
+      </c>
+      <c r="R34" s="14">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A35" s="7">
         <v>137</v>
       </c>
@@ -1704,8 +2423,38 @@
       <c r="I35" s="7">
         <v>8</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K35" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="L35" s="1">
+        <v>32</v>
+      </c>
+      <c r="M35" s="1">
+        <f>COUNTIF($B$2:$B$68,"y")</f>
+        <v>20</v>
+      </c>
+      <c r="N35" s="1">
+        <f>COUNTIFS($B$2:$B$66,"y", $H$2:$H$66,"&lt;&gt;0")</f>
+        <v>4</v>
+      </c>
+      <c r="O35" s="1">
+        <f>AVERAGEIFS($H$2:$H$66, $B$2:$B$66, "y", $H$2:$H$66, "&lt;&gt;0")</f>
+        <v>26.75</v>
+      </c>
+      <c r="P35" s="1">
+        <f>_xlfn.MINIFS($H$2:$H$66, $B$2:$B$66, "y", $H$2:$H$66, "&lt;&gt;0")</f>
+        <v>9</v>
+      </c>
+      <c r="Q35" s="1">
+        <f>_xlfn.MAXIFS($H$2:$H$66, $B$2:$B$66, "y", $H$2:$H$66, "&lt;&gt;0")</f>
+        <v>37</v>
+      </c>
+      <c r="R35" s="14">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A36" s="7">
         <v>141</v>
       </c>
@@ -1733,8 +2482,38 @@
       <c r="I36" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K36" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="L36" s="1">
+        <v>16</v>
+      </c>
+      <c r="M36" s="1">
+        <f>COUNTIF($B$2:$B$68,"r")</f>
+        <v>2</v>
+      </c>
+      <c r="N36" s="1">
+        <f>COUNTIFS($B$2:$B$66,"r", $H$2:$H$66,"&lt;&gt;0")</f>
+        <v>1</v>
+      </c>
+      <c r="O36" s="1">
+        <f>AVERAGEIFS($H$2:$H$66, $B$2:$B$66, "r", $H$2:$H$66, "&lt;&gt;0")</f>
+        <v>86</v>
+      </c>
+      <c r="P36" s="1">
+        <f>_xlfn.MINIFS($H$2:$H$66, $B$2:$B$66, "r", $H$2:$H$66, "&lt;&gt;0")</f>
+        <v>86</v>
+      </c>
+      <c r="Q36" s="1">
+        <f>_xlfn.MAXIFS($H$2:$H$66, $B$2:$B$66, "r", $H$2:$H$66, "&lt;&gt;0")</f>
+        <v>86</v>
+      </c>
+      <c r="R36" s="14">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A37" s="6">
         <v>94</v>
       </c>
@@ -1763,7 +2542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A38" s="9">
         <v>8</v>
       </c>
@@ -1791,8 +2570,18 @@
       <c r="I38" s="9">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K38" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="L38" s="13"/>
+      <c r="M38" s="13"/>
+      <c r="N38" s="13"/>
+      <c r="O38" s="13"/>
+      <c r="P38" s="13"/>
+      <c r="Q38" s="13"/>
+      <c r="R38" s="13"/>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>98</v>
       </c>
@@ -1820,8 +2609,32 @@
       <c r="I39" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K39" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L39" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M39" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N39" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O39" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P39" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q39" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R39" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A40" s="11">
         <v>11</v>
       </c>
@@ -1849,8 +2662,35 @@
       <c r="I40" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K40" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="L40" s="1">
+        <v>128</v>
+      </c>
+      <c r="M40" s="1">
+        <f>COUNTIF($B$2:$B$68,"o")</f>
+        <v>5</v>
+      </c>
+      <c r="N40" s="1">
+        <f>COUNTIFS($B$2:$B$66,"o", $I$2:$I$66,"&lt;&gt;0")</f>
+        <v>0</v>
+      </c>
+      <c r="O40" s="1">
+        <v>0</v>
+      </c>
+      <c r="P40" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q40" s="1">
+        <v>0</v>
+      </c>
+      <c r="R40" s="14">
+        <f>N40/M40*100</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A41" s="7">
         <v>82</v>
       </c>
@@ -1878,8 +2718,38 @@
       <c r="I41" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K41" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="L41" s="1">
+        <v>90</v>
+      </c>
+      <c r="M41" s="1">
+        <f>COUNTIF($B$2:$B$68,"w")</f>
+        <v>8</v>
+      </c>
+      <c r="N41" s="1">
+        <f>COUNTIFS($B$2:$B$66,"w", $I$2:$I$66,"&lt;&gt;0")</f>
+        <v>1</v>
+      </c>
+      <c r="O41" s="15">
+        <f>AVERAGEIFS($I$2:$I$66, $B$2:$B$66, "w", $I$2:$I$66, "&lt;&gt;0")</f>
+        <v>94</v>
+      </c>
+      <c r="P41" s="15">
+        <f>_xlfn.MINIFS($I$2:$I$66, $B$2:$B$66, "w", $I$2:$I$66, "&lt;&gt;0")</f>
+        <v>94</v>
+      </c>
+      <c r="Q41" s="15">
+        <f>_xlfn.MAXIFS($I$2:$I$66, $B$2:$B$66, "w", $I$2:$I$66, "&lt;&gt;0")</f>
+        <v>94</v>
+      </c>
+      <c r="R41" s="14">
+        <f t="shared" ref="R41:R45" si="4">N41/M41*100</f>
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A42" s="5">
         <v>18</v>
       </c>
@@ -1907,8 +2777,38 @@
       <c r="I42" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K42" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="L42" s="1">
+        <v>64</v>
+      </c>
+      <c r="M42" s="1">
+        <f>COUNTIF($B$2:$B$68,"p")</f>
+        <v>14</v>
+      </c>
+      <c r="N42" s="1">
+        <f>COUNTIFS($B$2:$B$66,"p", $I$2:$I$66,"&lt;&gt;0")</f>
+        <v>1</v>
+      </c>
+      <c r="O42" s="15">
+        <f>AVERAGEIFS($I$2:$I$66, $B$2:$B$66, "p", $I$2:$I$66, "&lt;&gt;0")</f>
+        <v>4</v>
+      </c>
+      <c r="P42" s="15">
+        <f>_xlfn.MINIFS($I$2:$I$66, $B$2:$B$66, "p", $I$2:$I$66, "&lt;&gt;0")</f>
+        <v>4</v>
+      </c>
+      <c r="Q42" s="15">
+        <f>_xlfn.MAXIFS($I$2:$I$66, $B$2:$B$66, "p", $I$2:$I$66, "&lt;&gt;0")</f>
+        <v>4</v>
+      </c>
+      <c r="R42" s="14">
+        <f t="shared" si="4"/>
+        <v>7.1428571428571423</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A43" s="7">
         <v>85</v>
       </c>
@@ -1936,8 +2836,38 @@
       <c r="I43" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K43" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L43" s="1">
+        <v>45</v>
+      </c>
+      <c r="M43" s="1">
+        <f>COUNTIF($B$2:$B$68,"g")</f>
+        <v>16</v>
+      </c>
+      <c r="N43" s="1">
+        <f>COUNTIFS($B$2:$B$66,"g", $I$2:$I$66,"&lt;&gt;0")</f>
+        <v>7</v>
+      </c>
+      <c r="O43" s="14">
+        <f>AVERAGEIFS($I$2:$I$66, $B$2:$B$66, "g", $I$2:$I$66, "&lt;&gt;0")</f>
+        <v>19.428571428571427</v>
+      </c>
+      <c r="P43" s="14">
+        <f>_xlfn.MINIFS($I$2:$I$66, $B$2:$B$66, "g", $I$2:$I$66, "&lt;&gt;0")</f>
+        <v>4</v>
+      </c>
+      <c r="Q43" s="14">
+        <f>_xlfn.MAXIFS($I$2:$I$66, $B$2:$B$66, "g", $I$2:$I$66, "&lt;&gt;0")</f>
+        <v>30</v>
+      </c>
+      <c r="R43" s="14">
+        <f t="shared" si="4"/>
+        <v>43.75</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>159</v>
       </c>
@@ -1965,8 +2895,38 @@
       <c r="I44" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K44" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="L44" s="1">
+        <v>32</v>
+      </c>
+      <c r="M44" s="1">
+        <f>COUNTIF($B$2:$B$68,"y")</f>
+        <v>20</v>
+      </c>
+      <c r="N44" s="1">
+        <f>COUNTIFS($B$2:$B$66,"y", $I$2:$I$66,"&lt;&gt;0")</f>
+        <v>6</v>
+      </c>
+      <c r="O44" s="14">
+        <f>AVERAGEIFS($I$2:$I$66, $B$2:$B$66, "y", $I$2:$I$66, "&lt;&gt;0")</f>
+        <v>107.83333333333333</v>
+      </c>
+      <c r="P44" s="14">
+        <f>_xlfn.MINIFS($I$2:$I$66, $B$2:$B$66, "y", $I$2:$I$66, "&lt;&gt;0")</f>
+        <v>2</v>
+      </c>
+      <c r="Q44" s="14">
+        <f>_xlfn.MAXIFS($I$2:$I$66, $B$2:$B$66, "y", $I$2:$I$66, "&lt;&gt;0")</f>
+        <v>534</v>
+      </c>
+      <c r="R44" s="14">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A45" s="5">
         <v>37</v>
       </c>
@@ -1994,8 +2954,38 @@
       <c r="I45" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K45" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="L45" s="1">
+        <v>16</v>
+      </c>
+      <c r="M45" s="1">
+        <f>COUNTIF($B$2:$B$68,"r")</f>
+        <v>2</v>
+      </c>
+      <c r="N45" s="1">
+        <f>COUNTIFS($B$2:$B$66,"r", $I$2:$I$66,"&lt;&gt;0")</f>
+        <v>1</v>
+      </c>
+      <c r="O45" s="15">
+        <f>AVERAGEIFS($I$2:$I$66, $B$2:$B$66, "r",$I$2:$I$66, "&lt;&gt;0")</f>
+        <v>95</v>
+      </c>
+      <c r="P45" s="15">
+        <f>_xlfn.MINIFS($I$2:$I$66, $B$2:$B$66, "r",$I$2:$I$66, "&lt;&gt;0")</f>
+        <v>95</v>
+      </c>
+      <c r="Q45" s="15">
+        <f>_xlfn.MAXIFS($I$2:$I$66, $B$2:$B$66, "r",$I$2:$I$66, "&lt;&gt;0")</f>
+        <v>95</v>
+      </c>
+      <c r="R45" s="14">
+        <f t="shared" si="4"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A46" s="7">
         <v>118</v>
       </c>
@@ -2024,7 +3014,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A47" s="12">
         <v>165</v>
       </c>
@@ -2053,7 +3043,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A48" s="4">
         <v>164</v>
       </c>
@@ -2082,7 +3072,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="9">
         <v>168</v>
       </c>
@@ -2111,7 +3101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="5">
         <v>17</v>
       </c>
@@ -2140,7 +3130,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" s="11">
         <v>150</v>
       </c>
@@ -2169,7 +3159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <v>132</v>
       </c>
@@ -2198,7 +3188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
         <v>161</v>
       </c>
@@ -2227,7 +3217,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" s="7">
         <v>145</v>
       </c>
@@ -2256,7 +3246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" s="2">
         <v>107</v>
       </c>
@@ -2285,7 +3275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" s="5">
         <v>105</v>
       </c>
@@ -2314,7 +3304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" s="2">
         <v>91</v>
       </c>
@@ -2343,7 +3333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" s="7">
         <v>69</v>
       </c>
@@ -2372,7 +3362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" s="11">
         <v>152</v>
       </c>
@@ -2401,7 +3391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" s="2">
         <v>121</v>
       </c>
@@ -2430,7 +3420,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" s="7">
         <v>61</v>
       </c>
@@ -2459,7 +3449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" s="7">
         <v>146</v>
       </c>
@@ -2488,7 +3478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" s="7">
         <v>45</v>
       </c>
@@ -2517,7 +3507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" s="7">
         <v>63</v>
       </c>
@@ -2546,7 +3536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" s="5">
         <v>96</v>
       </c>
@@ -2575,7 +3565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" s="5">
         <v>12</v>
       </c>
@@ -2604,7 +3594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" s="7">
         <v>74</v>
       </c>
@@ -2633,7 +3623,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" s="10">
         <v>51</v>
       </c>
@@ -2662,10 +3652,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="G69" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="K2:R2"/>
+    <mergeCell ref="K11:R11"/>
+    <mergeCell ref="K20:R20"/>
+    <mergeCell ref="K29:R29"/>
+    <mergeCell ref="K38:R38"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>